<commit_message>
Add Login pattern with test-data
</commit_message>
<xml_diff>
--- a/Data Files/Login/data_login.xlsx
+++ b/Data Files/Login/data_login.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -13,9 +13,29 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -32,7 +52,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,18 +60,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +150,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +185,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +393,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>